<commit_message>
Added FNE code of SAM and filtered the anomalous data from the original data
</commit_message>
<xml_diff>
--- a/Output_CSV/office_data/IF_anomaly_4h_9to6.xlsx
+++ b/Output_CSV/office_data/IF_anomaly_4h_9to6.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/mt5864s_login_missouristate_edu/Documents/Documents/Jupyter Notebooks/Thesis/Output_CSV/office_data/"/>
@@ -10,13 +10,29 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="8_{865A6EC5-9AD7-4B8C-A0EF-DAEC992777FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A13A26A8-B659-44E1-B9AE-B695BF9ED2A6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{BB59DA56-5F41-4D9B-B9E3-828D0630BCAD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{BB59DA56-5F41-4D9B-B9E3-828D0630BCAD}"/>
   </bookViews>
   <sheets>
     <sheet name="IF_anomaly_4H_9to6" sheetId="1" r:id="rId1"/>
     <sheet name="anomaly_aug-4H_9to6" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,10 +590,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -901,12 +913,12 @@
       <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -917,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>45475.5</v>
       </c>
@@ -928,7 +940,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>45475.666666666664</v>
       </c>
@@ -939,7 +951,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>45476.5</v>
       </c>
@@ -950,7 +962,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>45476.666666666664</v>
       </c>
@@ -961,7 +973,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>45477.5</v>
       </c>
@@ -972,7 +984,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>45477.666666666664</v>
       </c>
@@ -983,7 +995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>45478.5</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>45478.666666666664</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>45479.5</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>45479.666666666664</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>45480.5</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>45480.666666666664</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>45481.5</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>45481.666666666664</v>
       </c>
@@ -1071,7 +1083,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>45482.5</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>45482.666666666664</v>
       </c>
@@ -1093,7 +1105,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>45483.5</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>45483.666666666664</v>
       </c>
@@ -1115,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>45484.5</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>45484.666666666664</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>45485.5</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>45485.666666666664</v>
       </c>
@@ -1159,7 +1171,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>45486.5</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>45486.666666666664</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>45487.5</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>45487.666666666664</v>
       </c>
@@ -1203,7 +1215,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>45488.5</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>45488.666666666664</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>45489.5</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>45489.666666666664</v>
       </c>
@@ -1247,7 +1259,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>45490.5</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>45490.666666666664</v>
       </c>
@@ -1269,7 +1281,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>45491.5</v>
       </c>
@@ -1280,7 +1292,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>45491.666666666664</v>
       </c>
@@ -1291,7 +1303,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>45492.5</v>
       </c>
@@ -1302,7 +1314,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>45492.666666666664</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>45493.5</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>45493.666666666664</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>45494.5</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>45494.666666666664</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>45495.5</v>
       </c>
@@ -1368,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>45495.666666666664</v>
       </c>
@@ -1379,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>45496.5</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>45496.666666666664</v>
       </c>
@@ -1401,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>45497.5</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>45497.666666666664</v>
       </c>
@@ -1423,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>45498.5</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>45498.666666666664</v>
       </c>
@@ -1445,7 +1457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>45499.5</v>
       </c>
@@ -1456,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>45499.666666666664</v>
       </c>
@@ -1467,7 +1479,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>45500.5</v>
       </c>
@@ -1478,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>45500.666666666664</v>
       </c>
@@ -1489,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>45501.5</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>45501.666666666664</v>
       </c>
@@ -1511,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>45502.5</v>
       </c>
@@ -1522,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>45502.666666666664</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>45503.5</v>
       </c>
@@ -1544,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>45503.666666666664</v>
       </c>
@@ -1555,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>45504.5</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>45504.666666666664</v>
       </c>
@@ -1577,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>45505.5</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>45505.666666666664</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>45506.5</v>
       </c>
@@ -1610,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>45506.666666666664</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>45507.5</v>
       </c>
@@ -1632,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>45507.666666666664</v>
       </c>
@@ -1643,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>45508.5</v>
       </c>
@@ -1654,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>45508.666666666664</v>
       </c>
@@ -1665,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>45509.5</v>
       </c>
@@ -1676,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>45509.666666666664</v>
       </c>
@@ -1687,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>45510.5</v>
       </c>
@@ -1698,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>45510.666666666664</v>
       </c>
@@ -1709,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>45511.5</v>
       </c>
@@ -1720,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>45511.666666666664</v>
       </c>
@@ -1731,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>45512.5</v>
       </c>
@@ -1742,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>45512.666666666664</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>45513.5</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>45513.666666666664</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
         <v>45514.5</v>
       </c>
@@ -1786,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>45514.666666666664</v>
       </c>
@@ -1797,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>45515.5</v>
       </c>
@@ -1808,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>45515.666666666664</v>
       </c>
@@ -1819,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>45516.5</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>45516.666666666664</v>
       </c>
@@ -1841,7 +1853,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>45517.5</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>45517.666666666664</v>
       </c>
@@ -1863,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>45518.5</v>
       </c>
@@ -1874,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>45518.666666666664</v>
       </c>
@@ -1885,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>45519.5</v>
       </c>
@@ -1896,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>45519.666666666664</v>
       </c>
@@ -1907,7 +1919,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>45520.5</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>45520.666666666664</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>45521.5</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>45521.666666666664</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>45522.5</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>45522.666666666664</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="1">
         <v>45523.5</v>
       </c>
@@ -1984,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="1">
         <v>45523.666666666664</v>
       </c>
@@ -1995,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="1">
         <v>45524.5</v>
       </c>
@@ -2006,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="1">
         <v>45524.666666666664</v>
       </c>
@@ -2017,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" s="1">
         <v>45525.5</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" s="1">
         <v>45525.666666666664</v>
       </c>
@@ -2039,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" s="1">
         <v>45526.5</v>
       </c>
@@ -2050,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" s="1">
         <v>45526.666666666664</v>
       </c>
@@ -2061,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" s="1">
         <v>45527.5</v>
       </c>
@@ -2072,7 +2084,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" s="1">
         <v>45527.666666666664</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" s="1">
         <v>45528.5</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" s="1">
         <v>45528.666666666664</v>
       </c>
@@ -2105,7 +2117,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" s="1">
         <v>45529.5</v>
       </c>
@@ -2116,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" s="1">
         <v>45529.666666666664</v>
       </c>
@@ -2127,7 +2139,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" s="1">
         <v>45530.5</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" s="1">
         <v>45530.666666666664</v>
       </c>
@@ -2149,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" s="1">
         <v>45531.5</v>
       </c>
@@ -2160,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" s="1">
         <v>45531.666666666664</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" s="1">
         <v>45532.5</v>
       </c>
@@ -2182,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="1">
         <v>45532.666666666664</v>
       </c>
@@ -2193,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="1">
         <v>45533.5</v>
       </c>
@@ -2204,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="1">
         <v>45533.666666666664</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="1">
         <v>45534.5</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="1">
         <v>45534.666666666664</v>
       </c>
@@ -2237,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" s="1">
         <v>45535.5</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="1">
         <v>45535.666666666664</v>
       </c>
@@ -2259,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="1">
         <v>45536.5</v>
       </c>
@@ -2270,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="1">
         <v>45536.666666666664</v>
       </c>
@@ -2281,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="1">
         <v>45537.5</v>
       </c>
@@ -2292,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="1">
         <v>45537.666666666664</v>
       </c>
@@ -2303,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" s="1">
         <v>45538.5</v>
       </c>
@@ -2314,7 +2326,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" s="1">
         <v>45538.666666666664</v>
       </c>
@@ -2325,7 +2337,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" s="1">
         <v>45539.5</v>
       </c>
@@ -2336,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" s="1">
         <v>45539.666666666664</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" s="1">
         <v>45540.5</v>
       </c>
@@ -2358,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" s="1">
         <v>45540.666666666664</v>
       </c>
@@ -2369,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" s="1">
         <v>45541.5</v>
       </c>
@@ -2380,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" s="1">
         <v>45541.666666666664</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" s="1">
         <v>45542.5</v>
       </c>
@@ -2402,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" s="1">
         <v>45542.666666666664</v>
       </c>
@@ -2413,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" s="1">
         <v>45543.5</v>
       </c>
@@ -2424,7 +2436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" s="1">
         <v>45543.666666666664</v>
       </c>
@@ -2435,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3">
       <c r="A140" s="1">
         <v>45544.5</v>
       </c>
@@ -2446,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="A141" s="1">
         <v>45544.666666666664</v>
       </c>
@@ -2457,7 +2469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="A142" s="1">
         <v>45545.5</v>
       </c>
@@ -2468,7 +2480,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="A143" s="1">
         <v>45545.666666666664</v>
       </c>
@@ -2479,7 +2491,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" s="1">
         <v>45546.5</v>
       </c>
@@ -2490,7 +2502,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" s="1">
         <v>45546.666666666664</v>
       </c>
@@ -2501,7 +2513,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" s="1">
         <v>45547.5</v>
       </c>
@@ -2512,7 +2524,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" s="1">
         <v>45547.666666666664</v>
       </c>
@@ -2523,7 +2535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" s="1">
         <v>45548.5</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" s="1">
         <v>45548.666666666664</v>
       </c>
@@ -2545,7 +2557,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" s="1">
         <v>45549.5</v>
       </c>
@@ -2556,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" s="1">
         <v>45549.666666666664</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="A152" s="1">
         <v>45550.5</v>
       </c>
@@ -2578,7 +2590,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="A153" s="1">
         <v>45550.666666666664</v>
       </c>
@@ -2589,7 +2601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="A154" s="1">
         <v>45551.5</v>
       </c>
@@ -2600,7 +2612,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="A155" s="1">
         <v>45551.666666666664</v>
       </c>
@@ -2611,7 +2623,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="A156" s="1">
         <v>45552.5</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="A157" s="1">
         <v>45552.666666666664</v>
       </c>
@@ -2633,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="A158" s="1">
         <v>45553.5</v>
       </c>
@@ -2644,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" s="1">
         <v>45553.666666666664</v>
       </c>
@@ -2655,7 +2667,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" s="1">
         <v>45554.5</v>
       </c>
@@ -2666,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" s="1">
         <v>45554.666666666664</v>
       </c>
@@ -2677,7 +2689,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" s="1">
         <v>45555.5</v>
       </c>
@@ -2688,7 +2700,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" s="1">
         <v>45555.666666666664</v>
       </c>
@@ -2699,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" s="1">
         <v>45556.5</v>
       </c>
@@ -2710,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" s="1">
         <v>45556.666666666664</v>
       </c>
@@ -2721,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" s="1">
         <v>45557.5</v>
       </c>
@@ -2732,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" s="1">
         <v>45557.666666666664</v>
       </c>
@@ -2743,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3">
       <c r="A168" s="1">
         <v>45558.5</v>
       </c>
@@ -2754,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3">
       <c r="A169" s="1">
         <v>45558.666666666664</v>
       </c>
@@ -2765,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3">
       <c r="A170" s="1">
         <v>45559.5</v>
       </c>
@@ -2776,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3">
       <c r="A171" s="1">
         <v>45559.666666666664</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" s="1">
         <v>45560.5</v>
       </c>
@@ -2798,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" s="1">
         <v>45560.666666666664</v>
       </c>
@@ -2809,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" s="1">
         <v>45561.5</v>
       </c>
@@ -2820,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" s="1">
         <v>45561.666666666664</v>
       </c>
@@ -2831,7 +2843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" s="1">
         <v>45562.5</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3">
       <c r="A177" s="1">
         <v>45562.666666666664</v>
       </c>
@@ -2853,7 +2865,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3">
       <c r="A178" s="1">
         <v>45563.5</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3">
       <c r="A179" s="1">
         <v>45563.666666666664</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3">
       <c r="A180" s="1">
         <v>45564.5</v>
       </c>
@@ -2886,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3">
       <c r="A181" s="1">
         <v>45564.666666666664</v>
       </c>
@@ -2897,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3">
       <c r="A182" s="1">
         <v>45565.5</v>
       </c>
@@ -2908,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3">
       <c r="A183" s="1">
         <v>45565.666666666664</v>
       </c>
@@ -2919,7 +2931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3">
       <c r="A184" s="1">
         <v>45566.5</v>
       </c>
@@ -2930,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3">
       <c r="A185" s="1">
         <v>45566.666666666664</v>
       </c>
@@ -2966,12 +2978,12 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2982,7 +2994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>45516.666666666664</v>
       </c>
@@ -2993,7 +3005,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>45517.5</v>
       </c>
@@ -3004,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>45517.666666666664</v>
       </c>
@@ -3015,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>45518.5</v>
       </c>
@@ -3026,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>45518.666666666664</v>
       </c>
@@ -3037,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>45519.5</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>45519.666666666664</v>
       </c>
@@ -3059,7 +3071,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>45520.5</v>
       </c>
@@ -3070,7 +3082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>45520.666666666664</v>
       </c>
@@ -3081,7 +3093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>45521.5</v>
       </c>
@@ -3092,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>45521.666666666664</v>
       </c>
@@ -3103,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>45522.5</v>
       </c>
@@ -3114,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>45522.666666666664</v>
       </c>
@@ -3125,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>45523.5</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>45523.666666666664</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>45524.5</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>45524.666666666664</v>
       </c>
@@ -3169,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>45525.5</v>
       </c>
@@ -3180,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>45525.666666666664</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>45526.5</v>
       </c>
@@ -3202,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>45526.666666666664</v>
       </c>
@@ -3213,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>45527.5</v>
       </c>
@@ -3224,7 +3236,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>45527.666666666664</v>
       </c>
@@ -3235,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>45528.5</v>
       </c>
@@ -3246,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>45528.666666666664</v>
       </c>
@@ -3257,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>45529.5</v>
       </c>
@@ -3268,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>45529.666666666664</v>
       </c>
@@ -3279,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>45530.5</v>
       </c>
@@ -3290,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>45530.666666666664</v>
       </c>
@@ -3301,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>45531.5</v>
       </c>
@@ -3312,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>45531.666666666664</v>
       </c>
@@ -3323,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>45532.5</v>
       </c>
@@ -3334,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>45532.666666666664</v>
       </c>
@@ -3345,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>45533.5</v>
       </c>
@@ -3356,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>45533.666666666664</v>
       </c>
@@ -3367,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>45534.5</v>
       </c>
@@ -3378,7 +3390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>45534.666666666664</v>
       </c>
@@ -3389,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>45535.5</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>45535.666666666664</v>
       </c>
@@ -3411,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>45536.5</v>
       </c>
@@ -3422,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>45536.666666666664</v>
       </c>
@@ -3433,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>45537.5</v>
       </c>
@@ -3444,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>45537.666666666664</v>
       </c>
@@ -3455,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>45538.5</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>45538.666666666664</v>
       </c>
@@ -3477,7 +3489,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>45539.5</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>45539.666666666664</v>
       </c>
@@ -3499,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>45540.5</v>
       </c>
@@ -3510,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>45540.666666666664</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>45541.5</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>45541.666666666664</v>
       </c>
@@ -3543,7 +3555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>45542.5</v>
       </c>
@@ -3554,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>45542.666666666664</v>
       </c>
@@ -3565,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>45543.5</v>
       </c>
@@ -3576,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>45543.666666666664</v>
       </c>
@@ -3587,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>45544.5</v>
       </c>
@@ -3598,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>45544.666666666664</v>
       </c>
@@ -3609,7 +3621,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>45545.5</v>
       </c>
@@ -3620,7 +3632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>45545.666666666664</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>45546.5</v>
       </c>
@@ -3642,7 +3654,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>45546.666666666664</v>
       </c>
@@ -3653,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>45547.5</v>
       </c>
@@ -3664,7 +3676,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>45547.666666666664</v>
       </c>
@@ -3675,7 +3687,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>45548.5</v>
       </c>
@@ -3686,7 +3698,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>45548.666666666664</v>
       </c>
@@ -3697,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>45549.5</v>
       </c>
@@ -3708,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>45549.666666666664</v>
       </c>
@@ -3719,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>45550.5</v>
       </c>
@@ -3730,7 +3742,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>45550.666666666664</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>45551.5</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>45551.666666666664</v>
       </c>
@@ -3763,7 +3775,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>45552.5</v>
       </c>
@@ -3774,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>45552.666666666664</v>
       </c>
@@ -3785,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>45553.5</v>
       </c>
@@ -3796,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>45553.666666666664</v>
       </c>
@@ -3807,7 +3819,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>45554.5</v>
       </c>
@@ -3818,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>45554.666666666664</v>
       </c>
@@ -3829,7 +3841,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>45555.5</v>
       </c>
@@ -3840,7 +3852,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
         <v>45555.666666666664</v>
       </c>
@@ -3851,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>45556.5</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>45556.666666666664</v>
       </c>
@@ -3873,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>45557.5</v>
       </c>
@@ -3884,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>45557.666666666664</v>
       </c>
@@ -3895,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>45558.5</v>
       </c>
@@ -3906,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>45558.666666666664</v>
       </c>
@@ -3917,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>45559.5</v>
       </c>
@@ -3928,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>45559.666666666664</v>
       </c>
@@ -3939,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>45560.5</v>
       </c>
@@ -3950,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>45560.666666666664</v>
       </c>
@@ -3961,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>45561.5</v>
       </c>
@@ -3972,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>45561.666666666664</v>
       </c>
@@ -3983,7 +3995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>45562.5</v>
       </c>
@@ -3994,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>45562.666666666664</v>
       </c>
@@ -4005,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>45563.5</v>
       </c>
@@ -4016,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>45563.666666666664</v>
       </c>
@@ -4027,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>45564.5</v>
       </c>
@@ -4038,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="1">
         <v>45564.666666666664</v>
       </c>
@@ -4049,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="1">
         <v>45565.5</v>
       </c>
@@ -4060,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="1">
         <v>45565.666666666664</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="1">
         <v>45566.5</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" s="1">
         <v>45566.666666666664</v>
       </c>

</xml_diff>